<commit_message>
Code to check if any terms will be cancelled
</commit_message>
<xml_diff>
--- a/Spin_Boson/Calculation_Output.xlsx
+++ b/Spin_Boson/Calculation_Output.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EvaPei/Desktop/GT/Davidovic/TCL_GitHub_Access/Spin_Boson/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971D257B-64FF-5142-BC14-5EBC6DECBB0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C1651F-AA3C-DF4F-A90F-AD903BD2D90B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1414,8 +1427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D151"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1550,7 +1563,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="380" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="303" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -3303,5 +3316,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>